<commit_message>
Primeiro grafico e tabela autonomia
</commit_message>
<xml_diff>
--- a/relatorios/tabela testes consumo.xlsx
+++ b/relatorios/tabela testes consumo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Teste(nº)</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>100% uso do CPU</t>
+  </si>
+  <si>
+    <t>Equação utilizada para calcular as horas: =(360000/((0,133*F9)+G10+(75,233*F11)))/(3600/(F9+F10+F11))</t>
   </si>
 </sst>
 </file>
@@ -104,8 +107,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,20 +197,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -215,40 +209,52 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,668 +538,681 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="6"/>
-    <col min="3" max="3" width="10" style="6" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="6" customWidth="1"/>
-    <col min="6" max="9" width="10.7109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="6"/>
-    <col min="11" max="11" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="2.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="10" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="3" customWidth="1"/>
+    <col min="6" max="9" width="10.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="G3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="7">
         <v>100</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="7">
         <f>D4*3600</f>
         <v>360000</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="12"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="5" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
+      <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="9">
         <v>0.13300000000000001</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="10">
         <v>3540</v>
       </c>
-      <c r="G9" s="15">
-        <f>E9*F9</f>
+      <c r="G9" s="10">
+        <f>0.133*F9</f>
         <v>470.82000000000005</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <f>G9+G10+G11</f>
         <v>4984.8</v>
       </c>
-      <c r="I9" s="17">
-        <f>D$5/H9</f>
+      <c r="I9" s="16">
+        <f>360000/(G9+G10+G11)</f>
         <v>72.219547424169477</v>
       </c>
-      <c r="J9" s="17">
-        <f>I9/(3600/(F9+F10+F11))</f>
+      <c r="J9" s="16">
+        <f>(360000/((0.133*F9)+G10+(75.233*F11)))/(3600/(F9+F10+F11))</f>
         <v>72.219547424169477</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="17">
         <f>J9/24</f>
         <v>3.0091478093403947</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="11">
         <v>0</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="10">
         <v>0</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="10">
         <f>E10*F10</f>
         <v>0</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="11">
         <v>75.233000000000004</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="10">
         <v>60</v>
       </c>
-      <c r="G11" s="15">
-        <f t="shared" ref="G11" si="0">E11*F11</f>
+      <c r="G11" s="10">
+        <f>75.233*F11</f>
         <v>4513.9800000000005</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="7"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+      <c r="B13" s="18">
         <v>2</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="9">
         <v>0.13300000000000001</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="10">
         <v>3540</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="10">
         <f>E13*F13</f>
         <v>470.82000000000005</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <f>G13+G14+G15</f>
         <v>4756.8</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="16">
         <f>D$5/H13</f>
         <v>75.681130171543899</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="16">
         <f>I13/(3600/(F13+F14+F15))</f>
         <v>75.681130171543899</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="17">
         <f>J13/24</f>
         <v>3.1533804238143293</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="11">
         <v>0</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="10">
         <v>0</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="10">
         <f>E14*F14</f>
         <v>0</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="11">
         <v>71.433000000000007</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="10">
         <v>60</v>
       </c>
-      <c r="G15" s="15">
-        <f t="shared" ref="G15" si="1">E15*F15</f>
+      <c r="G15" s="10">
+        <f t="shared" ref="G15" si="0">E15*F15</f>
         <v>4285.9800000000005</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="18"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="7"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
+      <c r="B17" s="18">
         <v>3</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="9">
         <v>0.13300000000000001</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="10">
         <v>7190</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="10">
         <f>E17*F17</f>
         <v>956.2700000000001</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="15">
         <f>G17+G18+G19</f>
         <v>1670.6000000000001</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="16">
         <f>D$5/H17</f>
         <v>215.49144020112533</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="16">
         <f>I17/(3600/(F17+F18+F19))</f>
         <v>430.98288040225066</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="17">
         <f>J17/24</f>
         <v>17.957620016760444</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="11">
         <v>0</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="10">
         <v>0</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="10">
         <f>E18*F18</f>
         <v>0</v>
       </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="18"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="17"/>
     </row>
     <row r="19" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="11">
         <v>71.433000000000007</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="10">
         <v>10</v>
       </c>
-      <c r="G19" s="15">
-        <f t="shared" ref="G19" si="2">E19*F19</f>
+      <c r="G19" s="10">
+        <f t="shared" ref="G19" si="1">E19*F19</f>
         <v>714.33</v>
       </c>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="18"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="7"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
+      <c r="B21" s="18">
         <v>4</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="9">
         <v>0.13300000000000001</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="10">
         <v>7190</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="10">
         <f>E21*F21</f>
         <v>956.2700000000001</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="15">
         <f>G21+G22+G23</f>
         <v>1175.3030000000001</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="16">
         <f>D$5/H21</f>
         <v>306.30399139626121</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="16">
         <f>I21/(3600/(F21+F22+F23))</f>
         <v>612.60798279252242</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="17">
         <f>J21/24</f>
         <v>25.525332616355101</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="19"/>
+      <c r="C22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="11">
         <v>16.399999999999999</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="10">
         <v>9</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="10">
         <f>E22*F22</f>
         <v>147.6</v>
       </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="18"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="5" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="11">
         <v>71.433000000000007</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="10">
         <v>1</v>
       </c>
-      <c r="G23" s="15">
-        <f t="shared" ref="G23" si="3">E23*F23</f>
+      <c r="G23" s="10">
+        <f t="shared" ref="G23" si="2">E23*F23</f>
         <v>71.433000000000007</v>
       </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="18"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="17"/>
     </row>
     <row r="24" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="7"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="4"/>
     </row>
     <row r="25" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
+      <c r="B25" s="18">
         <v>5</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="9">
         <v>0.13300000000000001</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="10">
         <v>3590</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="10">
         <f>E25*F25</f>
         <v>477.47</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="15">
         <f>G25+G26+G27</f>
         <v>696.50300000000004</v>
       </c>
-      <c r="I25" s="17">
+      <c r="I25" s="16">
         <f>D$5/H25</f>
         <v>516.86783832948311</v>
       </c>
-      <c r="J25" s="17">
+      <c r="J25" s="16">
         <f>I25/(3600/(F25+F26+F27))</f>
         <v>516.86783832948311</v>
       </c>
-      <c r="K25" s="18">
+      <c r="K25" s="17">
         <f>J25/24</f>
         <v>21.536159930395129</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="5" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="11">
         <v>16.399999999999999</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="10">
         <v>9</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="10">
         <f>E26*F26</f>
         <v>147.6</v>
       </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="18"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="17"/>
     </row>
     <row r="27" spans="2:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="5" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="11">
         <v>71.433000000000007</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="10">
         <v>1</v>
       </c>
-      <c r="G27" s="15">
-        <f t="shared" ref="G27" si="4">E27*F27</f>
+      <c r="G27" s="10">
+        <f t="shared" ref="G27" si="3">E27*F27</f>
         <v>71.433000000000007</v>
       </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="18"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="17"/>
     </row>
     <row r="28" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
+      <c r="B29" s="18">
         <v>6</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="9">
         <v>0.13300000000000001</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="10">
         <v>3590</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="10">
         <f>E29*F29</f>
         <v>477.47</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="15">
         <f>G29+G30+G31</f>
         <v>1241.0030000000002</v>
       </c>
-      <c r="I29" s="17">
+      <c r="I29" s="16">
         <f>D$5/H29</f>
         <v>290.08793693488246</v>
       </c>
-      <c r="J29" s="17">
+      <c r="J29" s="16">
         <f>I29/(3600/(F29+F30+F31))</f>
         <v>290.08793693488246</v>
       </c>
-      <c r="K29" s="18">
+      <c r="K29" s="17">
         <f>J29/24</f>
         <v>12.086997372286769</v>
       </c>
     </row>
     <row r="30" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="5" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="11">
         <v>76.900000000000006</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="10">
         <v>9</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="10">
         <f>E30*F30</f>
         <v>692.1</v>
       </c>
-      <c r="H30" s="16"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="17"/>
     </row>
     <row r="31" spans="2:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="5" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="11">
         <v>71.433000000000007</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="10">
         <v>1</v>
       </c>
-      <c r="G31" s="15">
-        <f t="shared" ref="G31" si="5">E31*F31</f>
+      <c r="G31" s="10">
+        <f t="shared" ref="G31" si="4">E31*F31</f>
         <v>71.433000000000007</v>
       </c>
-      <c r="H31" s="16"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="18"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
+    <mergeCell ref="G3:K4"/>
     <mergeCell ref="K21:K23"/>
     <mergeCell ref="K17:K19"/>
     <mergeCell ref="B17:B19"/>
@@ -1205,7 +1224,6 @@
     <mergeCell ref="I29:I31"/>
     <mergeCell ref="J29:J31"/>
     <mergeCell ref="K29:K31"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="H25:H27"/>
     <mergeCell ref="I25:I27"/>
@@ -1215,12 +1233,13 @@
     <mergeCell ref="H21:H23"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K9:K11"/>
     <mergeCell ref="H13:H15"/>
     <mergeCell ref="I13:I15"/>
     <mergeCell ref="J13:J15"/>
     <mergeCell ref="K13:K15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="H9:H11"/>
     <mergeCell ref="H7:H8"/>
@@ -1232,8 +1251,8 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="F7:F8"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K9:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Grafico reformulado - relatorio, adicao das equacoes no relatorio e texto conclusivo
</commit_message>
<xml_diff>
--- a/relatorios/tabela testes consumo.xlsx
+++ b/relatorios/tabela testes consumo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="tabela consumo" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>100% uso do CPU</t>
   </si>
   <si>
-    <t>Equação utilizada para calcular as horas: =(360000/((0,133*F9)+G10+(75,233*F11)))/(3600/(F9+F10+F11))</t>
-  </si>
-  <si>
     <t>somatório consumo por ciclo</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Teste(nº) </t>
+  </si>
+  <si>
+    <t>Equação utilizada para calcular as horas: =(360000/((0,133*F9)+F10+(75,233*F11)))/(3600/(F9+F10+F11))</t>
   </si>
 </sst>
 </file>
@@ -295,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -374,6 +374,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -389,6 +392,9 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -396,21 +402,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -427,6 +418,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,7 +525,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.5843881099431895E-2"/>
+          <c:y val="0.11339616750479101"/>
+          <c:w val="0.90410250383092949"/>
+          <c:h val="0.74708693451348629"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -531,13 +544,10 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tabela grafico'!$G$7:$G$8</c:f>
+              <c:f>'tabela grafico'!$G$8</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Valor de bateria</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>teste 1</c:v>
                 </c:pt>
               </c:strCache>
@@ -586,7 +596,7 @@
                   <c:v>11064</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>-38784</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -603,13 +613,10 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tabela grafico'!$H$7:$H$8</c:f>
+              <c:f>'tabela grafico'!$H$8</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Valor de bateria</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>teste 2</c:v>
                 </c:pt>
               </c:strCache>
@@ -658,7 +665,7 @@
                   <c:v>27024</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>-20544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -675,13 +682,10 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tabela grafico'!$I$7:$I$8</c:f>
+              <c:f>'tabela grafico'!$I$8</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Valor de bateria</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>teste 3</c:v>
                 </c:pt>
               </c:strCache>
@@ -772,7 +776,7 @@
                   <c:v>9174</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>-7532.0000000000582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,13 +793,10 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tabela grafico'!$J$7:$J$8</c:f>
+              <c:f>'tabela grafico'!$J$8</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Valor de bateria</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>teste 4</c:v>
                 </c:pt>
               </c:strCache>
@@ -915,7 +916,7 @@
                   <c:v>7409.0999999999767</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>-4343.9300000000512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -932,13 +933,10 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tabela grafico'!$K$7:$K$8</c:f>
+              <c:f>'tabela grafico'!$K$8</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Valor de bateria</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>teste 5</c:v>
                 </c:pt>
               </c:strCache>
@@ -1121,7 +1119,7 @@
                   <c:v>4783.4699999999721</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
+                  <c:v>-2181.5599999999977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1138,13 +1136,10 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tabela grafico'!$L$7:$L$8</c:f>
+              <c:f>'tabela grafico'!$L$8</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Valor de bateria</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>teste 6</c:v>
                 </c:pt>
               </c:strCache>
@@ -1261,7 +1256,7 @@
                   <c:v>109.12999999994645</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>-12300.900000000023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1402,6 +1397,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="2"/>
         <c:tickMarkSkip val="5"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
@@ -1409,6 +1405,7 @@
         <c:axId val="1326557120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1521,6 +1518,64 @@
         <c:crossAx val="1326555040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="tenThousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1050"/>
+                    <a:t>x 10000</a:t>
+                  </a:r>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1530,6 +1585,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.74164721927249877"/>
+          <c:y val="0.1369721284839395"/>
+          <c:w val="0.12053073177033802"/>
+          <c:h val="0.38653752806186698"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2125,15 +2221,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>215152</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>6163</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>246530</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>25213</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2420,8 +2516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2440,23 +2536,23 @@
     <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
+      <c r="G3" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="4" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
@@ -2469,11 +2565,11 @@
       <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
     </row>
     <row r="5" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
@@ -2490,44 +2586,44 @@
     </row>
     <row r="6" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="30" t="s">
+      <c r="H7" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="30"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2536,7 +2632,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="30">
+      <c r="B9" s="31">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -2555,25 +2651,25 @@
         <f>0.133*F9</f>
         <v>470.82000000000005</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="33">
         <f>G9+G10+G11</f>
         <v>4984.8</v>
       </c>
-      <c r="I9" s="33">
-        <f>360000/(G9+G10+G11)</f>
+      <c r="I9" s="34">
+        <f>D$5/H9</f>
         <v>72.219547424169477</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="34">
         <f>(360000/((0.133*F9)+G10+(75.233*F11)))/(3600/(F9+F10+F11))</f>
         <v>72.219547424169477</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9" s="35">
         <f>J9/24</f>
         <v>3.0091478093403947</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="30"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
@@ -2590,13 +2686,13 @@
         <f>E10*F10</f>
         <v>0</v>
       </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="34"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="35"/>
     </row>
     <row r="11" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="30"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2613,10 +2709,10 @@
         <f>75.233*F11</f>
         <v>4513.9800000000005</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="34"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="35"/>
     </row>
     <row r="12" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
@@ -2631,7 +2727,7 @@
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="35">
+      <c r="B13" s="37">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -2650,25 +2746,25 @@
         <f>E13*F13</f>
         <v>470.82000000000005</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="33">
         <f>G13+G14+G15</f>
         <v>4756.8</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="34">
         <f>D$5/H13</f>
         <v>75.681130171543899</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="34">
         <f>I13/(3600/(F13+F14+F15))</f>
         <v>75.681130171543899</v>
       </c>
-      <c r="K13" s="34">
+      <c r="K13" s="35">
         <f>J13/24</f>
         <v>3.1533804238143293</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="36"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
@@ -2685,13 +2781,13 @@
         <f>E14*F14</f>
         <v>0</v>
       </c>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="34"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
@@ -2708,10 +2804,10 @@
         <f t="shared" ref="G15" si="0">E15*F15</f>
         <v>4285.9800000000005</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="34"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="35"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
@@ -2726,7 +2822,7 @@
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35">
+      <c r="B17" s="37">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -2745,25 +2841,25 @@
         <f>E17*F17</f>
         <v>956.2700000000001</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="33">
         <f>G17+G18+G19</f>
         <v>1670.6000000000001</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="34">
         <f>D$5/H17</f>
         <v>215.49144020112533</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="34">
         <f>I17/(3600/(F17+F18+F19))</f>
         <v>430.98288040225066</v>
       </c>
-      <c r="K17" s="34">
+      <c r="K17" s="35">
         <f>J17/24</f>
         <v>17.957620016760444</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="36"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
@@ -2780,13 +2876,13 @@
         <f>E18*F18</f>
         <v>0</v>
       </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="34"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="35"/>
     </row>
     <row r="19" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2803,10 +2899,10 @@
         <f t="shared" ref="G19" si="1">E19*F19</f>
         <v>714.33</v>
       </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="34"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="35"/>
     </row>
     <row r="20" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
@@ -2821,7 +2917,7 @@
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="35">
+      <c r="B21" s="37">
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -2840,25 +2936,25 @@
         <f>E21*F21</f>
         <v>956.2700000000001</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="33">
         <f>G21+G22+G23</f>
         <v>1175.3030000000001</v>
       </c>
-      <c r="I21" s="33">
+      <c r="I21" s="34">
         <f>D$5/H21</f>
         <v>306.30399139626121</v>
       </c>
-      <c r="J21" s="33">
+      <c r="J21" s="34">
         <f>I21/(3600/(F21+F22+F23))</f>
         <v>612.60798279252242</v>
       </c>
-      <c r="K21" s="34">
+      <c r="K21" s="35">
         <f>J21/24</f>
         <v>25.525332616355101</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="36"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="2" t="s">
         <v>5</v>
       </c>
@@ -2875,13 +2971,13 @@
         <f>E22*F22</f>
         <v>147.6</v>
       </c>
-      <c r="H22" s="32"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="34"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="35"/>
     </row>
     <row r="23" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="37"/>
+      <c r="B23" s="39"/>
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
@@ -2898,10 +2994,10 @@
         <f t="shared" ref="G23" si="2">E23*F23</f>
         <v>71.433000000000007</v>
       </c>
-      <c r="H23" s="32"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="34"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="35"/>
     </row>
     <row r="24" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
@@ -2916,7 +3012,7 @@
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="35">
+      <c r="B25" s="37">
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -2935,25 +3031,25 @@
         <f>E25*F25</f>
         <v>477.47</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="33">
         <f>G25+G26+G27</f>
         <v>696.50300000000004</v>
       </c>
-      <c r="I25" s="33">
+      <c r="I25" s="34">
         <f>D$5/H25</f>
         <v>516.86783832948311</v>
       </c>
-      <c r="J25" s="33">
+      <c r="J25" s="34">
         <f>I25/(3600/(F25+F26+F27))</f>
         <v>516.86783832948311</v>
       </c>
-      <c r="K25" s="34">
+      <c r="K25" s="35">
         <f>J25/24</f>
         <v>21.536159930395129</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="36"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="2" t="s">
         <v>5</v>
       </c>
@@ -2970,13 +3066,13 @@
         <f>E26*F26</f>
         <v>147.6</v>
       </c>
-      <c r="H26" s="32"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="34"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="35"/>
     </row>
     <row r="27" spans="2:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="37"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
@@ -2993,10 +3089,10 @@
         <f t="shared" ref="G27" si="3">E27*F27</f>
         <v>71.433000000000007</v>
       </c>
-      <c r="H27" s="32"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="34"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="35"/>
     </row>
     <row r="28" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
@@ -3011,7 +3107,7 @@
       <c r="K28" s="6"/>
     </row>
     <row r="29" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="35">
+      <c r="B29" s="37">
         <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -3030,25 +3126,25 @@
         <f>E29*F29</f>
         <v>477.47</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="33">
         <f>G29+G30+G31</f>
         <v>1241.0030000000002</v>
       </c>
-      <c r="I29" s="33">
+      <c r="I29" s="34">
         <f>D$5/H29</f>
         <v>290.08793693488246</v>
       </c>
-      <c r="J29" s="33">
+      <c r="J29" s="34">
         <f>I29/(3600/(F29+F30+F31))</f>
         <v>290.08793693488246</v>
       </c>
-      <c r="K29" s="34">
+      <c r="K29" s="35">
         <f>J29/24</f>
         <v>12.086997372286769</v>
       </c>
     </row>
     <row r="30" spans="2:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="2" t="s">
         <v>5</v>
       </c>
@@ -3065,13 +3161,13 @@
         <f>E30*F30</f>
         <v>692.1</v>
       </c>
-      <c r="H30" s="32"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="34"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="35"/>
     </row>
     <row r="31" spans="2:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="37"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="2" t="s">
         <v>7</v>
       </c>
@@ -3088,10 +3184,10 @@
         <f t="shared" ref="G31" si="4">E31*F31</f>
         <v>71.433000000000007</v>
       </c>
-      <c r="H31" s="32"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="34"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="41">
@@ -3146,8 +3242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3163,10 +3259,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="47"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="24"/>
       <c r="E3" s="16"/>
       <c r="F3" s="22"/>
@@ -3176,7 +3272,7 @@
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="29">
         <v>100</v>
@@ -3192,7 +3288,7 @@
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="27">
         <f>C4* 3600</f>
@@ -3204,151 +3300,151 @@
     </row>
     <row r="6" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="35" t="s">
+      <c r="B7" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="39" t="s">
+      <c r="G7" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+    </row>
+    <row r="8" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-    </row>
-    <row r="8" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="27" t="s">
+      <c r="H8" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="I8" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="J8" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="K8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="27" t="s">
-        <v>33</v>
-      </c>
       <c r="L8" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="35">
+      <c r="B9" s="37">
         <v>1</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="40">
         <f>'tabela consumo'!H9:H11</f>
         <v>4984.8</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="41"/>
+      <c r="E9" s="47"/>
       <c r="F9" s="27">
         <v>0</v>
       </c>
       <c r="G9" s="27">
-        <f>IF($C$5 - ($F9*$C$9) &gt; 0, $C$5 - ($F9*$C$9), 0)</f>
+        <f>$C$5 - ($F9*$C$9)</f>
         <v>360000</v>
       </c>
       <c r="H9" s="27">
-        <f>IF($C$5 - ($F9*$C$13) &gt; 0, $C$5 - ($F9*$C$13), 0)</f>
+        <f>$C$5 - ($F9*$C$13)</f>
         <v>360000</v>
       </c>
       <c r="I9" s="27">
-        <f>IF($C$5 - ($F9*$C$17) &gt; 0, $C$5 - ($F9*$C$17), 0)</f>
+        <f>$C$5 - ($F9*$C$17)</f>
         <v>360000</v>
       </c>
       <c r="J9" s="27">
-        <f>IF($C$5 - ($F9*$C$21) &gt; 0, $C$5 - ($F9*$C$21), 0)</f>
+        <f>$C$5 - ($F9*$C$21)</f>
         <v>360000</v>
       </c>
       <c r="K9" s="27">
-        <f>IF($C$5 - ($F9*$C$25) &gt; 0, $C$5 - ($F9*$C$25), 0)</f>
+        <f>$C$5 - ($F9*$C$25)</f>
         <v>360000</v>
       </c>
       <c r="L9" s="27">
-        <f>IF($C$5 - ($F9*$C$29) &gt; 0, $C$5 - ($F9*$C$29), 0)</f>
+        <f>$C$5 - ($F9*$C$29)*2</f>
         <v>360000</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36"/>
-      <c r="C10" s="44"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="18"/>
-      <c r="E10" s="41"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="27">
         <v>10</v>
       </c>
-      <c r="G10" s="27">
-        <f t="shared" ref="G10:G17" si="0">IF($C$5 - ($F10*$C$9) &gt; 0, $C$5 - ($F10*$C$9), 0)</f>
+      <c r="G10" s="30">
+        <f t="shared" ref="G10:G17" si="0">$C$5 - ($F10*$C$9)</f>
         <v>310152</v>
       </c>
-      <c r="H10" s="27">
-        <f t="shared" ref="H10:H17" si="1">IF($C$5 - ($F10*$C$13) &gt; 0, $C$5 - ($F10*$C$13), 0)</f>
+      <c r="H10" s="30">
+        <f t="shared" ref="H10:H17" si="1">$C$5 - ($F10*$C$13)</f>
         <v>312432</v>
       </c>
-      <c r="I10" s="27">
-        <f t="shared" ref="I10:I31" si="2">IF($C$5 - ($F10*$C$17) &gt; 0, $C$5 - ($F10*$C$17), 0)</f>
+      <c r="I10" s="30">
+        <f t="shared" ref="I10:I31" si="2">$C$5 - ($F10*$C$17)</f>
         <v>343294</v>
       </c>
-      <c r="J10" s="27">
-        <f t="shared" ref="J10:J40" si="3">IF($C$5 - ($F10*$C$21) &gt; 0, $C$5 - ($F10*$C$21), 0)</f>
+      <c r="J10" s="30">
+        <f t="shared" ref="J10:J40" si="3">$C$5 - ($F10*$C$21)</f>
         <v>348246.97</v>
       </c>
-      <c r="K10" s="27">
-        <f t="shared" ref="K10:K61" si="4">IF($C$5 - ($F10*$C$25) &gt; 0, $C$5 - ($F10*$C$25), 0)</f>
+      <c r="K10" s="30">
+        <f t="shared" ref="K10:K61" si="4">$C$5 - ($F10*$C$25)</f>
         <v>353034.97</v>
       </c>
-      <c r="L10" s="27">
-        <f t="shared" ref="L10:L39" si="5">IF($C$5 - ($F10*$C$29) &gt; 0, $C$5 - ($F10*$C$29), 0)</f>
+      <c r="L10" s="30">
+        <f t="shared" ref="L10:L39" si="5">$C$5 - ($F10*$C$29)</f>
         <v>347589.97</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="37"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="18"/>
-      <c r="E11" s="41"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="27">
         <v>20</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="30">
         <f t="shared" si="0"/>
         <v>260304</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="30">
         <f t="shared" si="1"/>
         <v>264864</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="30">
         <f t="shared" si="2"/>
         <v>326588</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11" s="30">
         <f t="shared" si="3"/>
         <v>336493.94</v>
       </c>
-      <c r="K11" s="27">
+      <c r="K11" s="30">
         <f t="shared" si="4"/>
         <v>346069.94</v>
       </c>
-      <c r="L11" s="27">
+      <c r="L11" s="30">
         <f t="shared" si="5"/>
         <v>335179.94</v>
       </c>
@@ -3357,135 +3453,135 @@
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="41"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="27">
         <v>30</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="30">
         <f t="shared" si="0"/>
         <v>210456</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="30">
         <f t="shared" si="1"/>
         <v>217296</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I12" s="30">
         <f t="shared" si="2"/>
         <v>309882</v>
       </c>
-      <c r="J12" s="27">
+      <c r="J12" s="30">
         <f t="shared" si="3"/>
         <v>324740.90999999997</v>
       </c>
-      <c r="K12" s="27">
+      <c r="K12" s="30">
         <f t="shared" si="4"/>
         <v>339104.91</v>
       </c>
-      <c r="L12" s="27">
+      <c r="L12" s="30">
         <f t="shared" si="5"/>
         <v>322769.90999999997</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="35">
+      <c r="B13" s="37">
         <v>2</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="40">
         <f>'tabela consumo'!$H$9:H13</f>
         <v>4756.8</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="41"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="27">
         <v>40</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>160608</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="30">
         <f t="shared" si="1"/>
         <v>169728</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="30">
         <f t="shared" si="2"/>
         <v>293176</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13" s="30">
         <f t="shared" si="3"/>
         <v>312987.88</v>
       </c>
-      <c r="K13" s="27">
+      <c r="K13" s="30">
         <f t="shared" si="4"/>
         <v>332139.88</v>
       </c>
-      <c r="L13" s="27">
+      <c r="L13" s="30">
         <f t="shared" si="5"/>
         <v>310359.88</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="36"/>
-      <c r="C14" s="44"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="41"/>
+      <c r="E14" s="47"/>
       <c r="F14" s="27">
         <v>50</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>110760</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="30">
         <f t="shared" si="1"/>
         <v>122160</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="30">
         <f t="shared" si="2"/>
         <v>276470</v>
       </c>
-      <c r="J14" s="27">
+      <c r="J14" s="30">
         <f t="shared" si="3"/>
         <v>301234.84999999998</v>
       </c>
-      <c r="K14" s="27">
+      <c r="K14" s="30">
         <f t="shared" si="4"/>
         <v>325174.84999999998</v>
       </c>
-      <c r="L14" s="27">
+      <c r="L14" s="30">
         <f t="shared" si="5"/>
         <v>297949.84999999998</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="45"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="18"/>
-      <c r="E15" s="41"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="27">
         <v>60</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="30">
         <f t="shared" si="0"/>
         <v>60912</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="30">
         <f t="shared" si="1"/>
         <v>74592</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="30">
         <f t="shared" si="2"/>
         <v>259764</v>
       </c>
-      <c r="J15" s="27">
+      <c r="J15" s="30">
         <f t="shared" si="3"/>
         <v>289481.82</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K15" s="30">
         <f t="shared" si="4"/>
         <v>318209.82</v>
       </c>
-      <c r="L15" s="27">
+      <c r="L15" s="30">
         <f t="shared" si="5"/>
         <v>285539.82</v>
       </c>
@@ -3494,123 +3590,123 @@
       <c r="B16" s="15"/>
       <c r="C16" s="14"/>
       <c r="D16" s="18"/>
-      <c r="E16" s="41"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="27">
         <v>70</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="30">
         <f t="shared" si="0"/>
         <v>11064</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="30">
         <f t="shared" si="1"/>
         <v>27024</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="30">
         <f t="shared" si="2"/>
         <v>243058</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J16" s="30">
         <f t="shared" si="3"/>
         <v>277728.78999999998</v>
       </c>
-      <c r="K16" s="27">
+      <c r="K16" s="30">
         <f t="shared" si="4"/>
         <v>311244.78999999998</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="30">
         <f t="shared" si="5"/>
         <v>273129.78999999998</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="35">
+      <c r="B17" s="37">
         <v>3</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="40">
         <f>'tabela consumo'!$H$9:H17</f>
         <v>1670.6000000000001</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="41"/>
+      <c r="E17" s="47"/>
       <c r="F17" s="27">
         <v>80</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="27">
+        <v>-38784</v>
+      </c>
+      <c r="H17" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="27">
+        <v>-20544</v>
+      </c>
+      <c r="I17" s="30">
         <f t="shared" si="2"/>
         <v>226352</v>
       </c>
-      <c r="J17" s="27">
+      <c r="J17" s="30">
         <f t="shared" si="3"/>
         <v>265975.76</v>
       </c>
-      <c r="K17" s="27">
+      <c r="K17" s="30">
         <f t="shared" si="4"/>
         <v>304279.76</v>
       </c>
-      <c r="L17" s="27">
+      <c r="L17" s="30">
         <f t="shared" si="5"/>
         <v>260719.75999999998</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="44"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="41"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="41"/>
+      <c r="E18" s="47"/>
       <c r="F18" s="27">
         <v>90</v>
       </c>
-      <c r="G18" s="27"/>
+      <c r="G18" s="30"/>
       <c r="H18" s="27"/>
-      <c r="I18" s="27">
+      <c r="I18" s="30">
         <f t="shared" si="2"/>
         <v>209646</v>
       </c>
-      <c r="J18" s="27">
+      <c r="J18" s="30">
         <f t="shared" si="3"/>
         <v>254222.72999999998</v>
       </c>
-      <c r="K18" s="27">
+      <c r="K18" s="30">
         <f t="shared" si="4"/>
         <v>297314.73</v>
       </c>
-      <c r="L18" s="27">
+      <c r="L18" s="30">
         <f t="shared" si="5"/>
         <v>248309.72999999998</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="45"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="41"/>
+      <c r="E19" s="47"/>
       <c r="F19" s="27">
         <v>100</v>
       </c>
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
-      <c r="I19" s="27">
+      <c r="I19" s="30">
         <f t="shared" si="2"/>
         <v>192940</v>
       </c>
-      <c r="J19" s="27">
+      <c r="J19" s="30">
         <f t="shared" si="3"/>
         <v>242469.69999999998</v>
       </c>
-      <c r="K19" s="27">
+      <c r="K19" s="30">
         <f t="shared" si="4"/>
         <v>290349.7</v>
       </c>
-      <c r="L19" s="27">
+      <c r="L19" s="30">
         <f t="shared" si="5"/>
         <v>235899.69999999998</v>
       </c>
@@ -3619,111 +3715,111 @@
       <c r="B20" s="15"/>
       <c r="C20" s="14"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="41"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="27">
         <v>110</v>
       </c>
       <c r="G20" s="27"/>
       <c r="H20" s="27"/>
-      <c r="I20" s="27">
+      <c r="I20" s="30">
         <f t="shared" si="2"/>
         <v>176233.99999999997</v>
       </c>
-      <c r="J20" s="27">
+      <c r="J20" s="30">
         <f t="shared" si="3"/>
         <v>230716.66999999998</v>
       </c>
-      <c r="K20" s="27">
+      <c r="K20" s="30">
         <f t="shared" si="4"/>
         <v>283384.67</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L20" s="30">
         <f t="shared" si="5"/>
         <v>223489.66999999998</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="35">
+      <c r="B21" s="37">
         <v>4</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="40">
         <f>'tabela consumo'!$H$9:H21</f>
         <v>1175.3030000000001</v>
       </c>
       <c r="D21" s="18"/>
-      <c r="E21" s="41"/>
+      <c r="E21" s="47"/>
       <c r="F21" s="27">
         <v>120</v>
       </c>
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
-      <c r="I21" s="27">
+      <c r="I21" s="30">
         <f t="shared" si="2"/>
         <v>159527.99999999997</v>
       </c>
-      <c r="J21" s="27">
+      <c r="J21" s="30">
         <f t="shared" si="3"/>
         <v>218963.63999999998</v>
       </c>
-      <c r="K21" s="27">
+      <c r="K21" s="30">
         <f t="shared" si="4"/>
         <v>276419.64</v>
       </c>
-      <c r="L21" s="27">
+      <c r="L21" s="30">
         <f t="shared" si="5"/>
         <v>211079.63999999998</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="36"/>
-      <c r="C22" s="44"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="41"/>
+      <c r="E22" s="47"/>
       <c r="F22" s="27">
         <v>130</v>
       </c>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
-      <c r="I22" s="27">
+      <c r="I22" s="30">
         <f t="shared" si="2"/>
         <v>142821.99999999997</v>
       </c>
-      <c r="J22" s="27">
+      <c r="J22" s="30">
         <f t="shared" si="3"/>
         <v>207210.61</v>
       </c>
-      <c r="K22" s="27">
-        <f>IF($C$5 - ($F22*$C$25) &gt; 0, $C$5 - ($F22*$C$25), 0)</f>
+      <c r="K22" s="30">
+        <f t="shared" si="4"/>
         <v>269454.61</v>
       </c>
-      <c r="L22" s="27">
+      <c r="L22" s="30">
         <f t="shared" si="5"/>
         <v>198669.61</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="37"/>
-      <c r="C23" s="45"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="41"/>
+      <c r="E23" s="47"/>
       <c r="F23" s="27">
         <v>140</v>
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
-      <c r="I23" s="27">
+      <c r="I23" s="30">
         <f t="shared" si="2"/>
         <v>126115.99999999997</v>
       </c>
-      <c r="J23" s="27">
+      <c r="J23" s="30">
         <f t="shared" si="3"/>
         <v>195457.58</v>
       </c>
-      <c r="K23" s="27">
+      <c r="K23" s="30">
         <f t="shared" si="4"/>
         <v>262489.57999999996</v>
       </c>
-      <c r="L23" s="27">
+      <c r="L23" s="30">
         <f t="shared" si="5"/>
         <v>186259.58</v>
       </c>
@@ -3732,111 +3828,111 @@
       <c r="B24" s="13"/>
       <c r="C24" s="11"/>
       <c r="D24" s="19"/>
-      <c r="E24" s="41"/>
+      <c r="E24" s="47"/>
       <c r="F24" s="27">
         <v>150</v>
       </c>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
-      <c r="I24" s="27">
+      <c r="I24" s="30">
         <f t="shared" si="2"/>
         <v>109409.99999999997</v>
       </c>
-      <c r="J24" s="27">
+      <c r="J24" s="30">
         <f t="shared" si="3"/>
         <v>183704.55</v>
       </c>
-      <c r="K24" s="27">
+      <c r="K24" s="30">
         <f t="shared" si="4"/>
         <v>255524.55</v>
       </c>
-      <c r="L24" s="27">
+      <c r="L24" s="30">
         <f t="shared" si="5"/>
         <v>173849.55</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="35">
+      <c r="B25" s="37">
         <v>5</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="40">
         <f>'tabela consumo'!$H$9:H25</f>
         <v>696.50300000000004</v>
       </c>
       <c r="D25" s="18"/>
-      <c r="E25" s="41"/>
+      <c r="E25" s="47"/>
       <c r="F25" s="27">
         <v>160</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="28"/>
-      <c r="I25" s="27">
+      <c r="I25" s="30">
         <f t="shared" si="2"/>
         <v>92704</v>
       </c>
-      <c r="J25" s="27">
+      <c r="J25" s="30">
         <f t="shared" si="3"/>
         <v>171951.52</v>
       </c>
-      <c r="K25" s="27">
+      <c r="K25" s="30">
         <f t="shared" si="4"/>
         <v>248559.52</v>
       </c>
-      <c r="L25" s="27">
+      <c r="L25" s="30">
         <f t="shared" si="5"/>
         <v>161439.51999999996</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="36"/>
-      <c r="C26" s="44"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="41"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="41"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="27">
         <v>170</v>
       </c>
       <c r="G26" s="27"/>
       <c r="H26" s="28"/>
-      <c r="I26" s="27">
+      <c r="I26" s="30">
         <f t="shared" si="2"/>
         <v>75998</v>
       </c>
-      <c r="J26" s="27">
+      <c r="J26" s="30">
         <f t="shared" si="3"/>
         <v>160198.49</v>
       </c>
-      <c r="K26" s="27">
+      <c r="K26" s="30">
         <f t="shared" si="4"/>
         <v>241594.49</v>
       </c>
-      <c r="L26" s="27">
+      <c r="L26" s="30">
         <f t="shared" si="5"/>
         <v>149029.48999999996</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="37"/>
-      <c r="C27" s="45"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="41"/>
+      <c r="E27" s="47"/>
       <c r="F27" s="27">
         <v>180</v>
       </c>
       <c r="G27" s="27"/>
       <c r="H27" s="28"/>
-      <c r="I27" s="27">
+      <c r="I27" s="30">
         <f t="shared" si="2"/>
         <v>59292</v>
       </c>
-      <c r="J27" s="27">
+      <c r="J27" s="30">
         <f t="shared" si="3"/>
         <v>148445.46</v>
       </c>
-      <c r="K27" s="27">
+      <c r="K27" s="30">
         <f t="shared" si="4"/>
         <v>234629.46</v>
       </c>
-      <c r="L27" s="27">
+      <c r="L27" s="30">
         <f t="shared" si="5"/>
         <v>136619.45999999996</v>
       </c>
@@ -3845,303 +3941,303 @@
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="20"/>
-      <c r="E28" s="41"/>
+      <c r="E28" s="47"/>
       <c r="F28" s="27">
         <v>190</v>
       </c>
       <c r="G28" s="27"/>
       <c r="H28" s="28"/>
-      <c r="I28" s="27">
+      <c r="I28" s="30">
         <f t="shared" si="2"/>
         <v>42586</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J28" s="30">
         <f t="shared" si="3"/>
         <v>136692.43</v>
       </c>
-      <c r="K28" s="27">
+      <c r="K28" s="30">
         <f t="shared" si="4"/>
         <v>227664.43</v>
       </c>
-      <c r="L28" s="27">
+      <c r="L28" s="30">
         <f t="shared" si="5"/>
         <v>124209.42999999996</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="35">
+      <c r="B29" s="37">
         <v>6</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="40">
         <f>'tabela consumo'!$H$9:H29</f>
         <v>1241.0030000000002</v>
       </c>
       <c r="D29" s="18"/>
-      <c r="E29" s="41"/>
+      <c r="E29" s="47"/>
       <c r="F29" s="27">
         <v>200</v>
       </c>
       <c r="G29" s="27"/>
       <c r="H29" s="28"/>
-      <c r="I29" s="27">
+      <c r="I29" s="30">
         <f t="shared" si="2"/>
         <v>25880</v>
       </c>
-      <c r="J29" s="27">
+      <c r="J29" s="30">
         <f t="shared" si="3"/>
         <v>124939.39999999997</v>
       </c>
-      <c r="K29" s="27">
+      <c r="K29" s="30">
         <f t="shared" si="4"/>
         <v>220699.4</v>
       </c>
-      <c r="L29" s="27">
+      <c r="L29" s="30">
         <f t="shared" si="5"/>
         <v>111799.39999999997</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="36"/>
-      <c r="C30" s="44"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="41"/>
       <c r="D30" s="18"/>
-      <c r="E30" s="41"/>
+      <c r="E30" s="47"/>
       <c r="F30" s="27">
         <v>210</v>
       </c>
       <c r="G30" s="27"/>
       <c r="H30" s="28"/>
-      <c r="I30" s="27">
+      <c r="I30" s="30">
         <f t="shared" si="2"/>
         <v>9174</v>
       </c>
-      <c r="J30" s="27">
+      <c r="J30" s="30">
         <f t="shared" si="3"/>
         <v>113186.36999999997</v>
       </c>
-      <c r="K30" s="27">
+      <c r="K30" s="30">
         <f t="shared" si="4"/>
         <v>213734.37</v>
       </c>
-      <c r="L30" s="27">
+      <c r="L30" s="30">
         <f t="shared" si="5"/>
         <v>99389.369999999966</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="37"/>
-      <c r="C31" s="45"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="42"/>
       <c r="D31" s="18"/>
-      <c r="E31" s="41"/>
+      <c r="E31" s="47"/>
       <c r="F31" s="27">
         <v>220</v>
       </c>
       <c r="G31" s="27"/>
       <c r="H31" s="28"/>
-      <c r="I31" s="27">
+      <c r="I31" s="30">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J31" s="27">
+        <v>-7532.0000000000582</v>
+      </c>
+      <c r="J31" s="30">
         <f t="shared" si="3"/>
         <v>101433.33999999997</v>
       </c>
-      <c r="K31" s="27">
+      <c r="K31" s="30">
         <f t="shared" si="4"/>
         <v>206769.34</v>
       </c>
-      <c r="L31" s="27">
+      <c r="L31" s="30">
         <f t="shared" si="5"/>
         <v>86979.339999999967</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E32" s="41"/>
+      <c r="E32" s="47"/>
       <c r="F32" s="27">
         <v>230</v>
       </c>
       <c r="G32" s="27"/>
       <c r="H32" s="28"/>
       <c r="I32" s="27"/>
-      <c r="J32" s="27">
+      <c r="J32" s="30">
         <f t="shared" si="3"/>
         <v>89680.31</v>
       </c>
-      <c r="K32" s="27">
+      <c r="K32" s="30">
         <f t="shared" si="4"/>
         <v>199804.31</v>
       </c>
-      <c r="L32" s="27">
+      <c r="L32" s="30">
         <f t="shared" si="5"/>
         <v>74569.309999999939</v>
       </c>
     </row>
     <row r="33" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E33" s="41"/>
+      <c r="E33" s="47"/>
       <c r="F33" s="27">
         <v>240</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="28"/>
       <c r="I33" s="27"/>
-      <c r="J33" s="27">
+      <c r="J33" s="30">
         <f t="shared" si="3"/>
         <v>77927.27999999997</v>
       </c>
-      <c r="K33" s="27">
+      <c r="K33" s="30">
         <f t="shared" si="4"/>
         <v>192839.28</v>
       </c>
-      <c r="L33" s="27">
+      <c r="L33" s="30">
         <f t="shared" si="5"/>
         <v>62159.27999999997</v>
       </c>
     </row>
     <row r="34" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E34" s="41"/>
+      <c r="E34" s="47"/>
       <c r="F34" s="27">
         <v>250</v>
       </c>
       <c r="G34" s="27"/>
       <c r="H34" s="28"/>
       <c r="I34" s="27"/>
-      <c r="J34" s="27">
+      <c r="J34" s="30">
         <f t="shared" si="3"/>
         <v>66174.25</v>
       </c>
-      <c r="K34" s="27">
+      <c r="K34" s="30">
         <f t="shared" si="4"/>
         <v>185874.25</v>
       </c>
-      <c r="L34" s="27">
+      <c r="L34" s="30">
         <f t="shared" si="5"/>
         <v>49749.249999999942</v>
       </c>
     </row>
     <row r="35" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E35" s="41"/>
+      <c r="E35" s="47"/>
       <c r="F35" s="27">
         <v>260</v>
       </c>
       <c r="G35" s="27"/>
       <c r="H35" s="28"/>
       <c r="I35" s="27"/>
-      <c r="J35" s="27">
+      <c r="J35" s="30">
         <f t="shared" si="3"/>
         <v>54421.219999999972</v>
       </c>
-      <c r="K35" s="27">
+      <c r="K35" s="30">
         <f t="shared" si="4"/>
         <v>178909.22</v>
       </c>
-      <c r="L35" s="27">
+      <c r="L35" s="30">
         <f t="shared" si="5"/>
         <v>37339.219999999972</v>
       </c>
     </row>
     <row r="36" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E36" s="41"/>
+      <c r="E36" s="47"/>
       <c r="F36" s="27">
         <v>270</v>
       </c>
       <c r="G36" s="27"/>
       <c r="H36" s="28"/>
       <c r="I36" s="27"/>
-      <c r="J36" s="27">
+      <c r="J36" s="30">
         <f t="shared" si="3"/>
         <v>42668.189999999944</v>
       </c>
-      <c r="K36" s="27">
+      <c r="K36" s="30">
         <f t="shared" si="4"/>
         <v>171944.19</v>
       </c>
-      <c r="L36" s="27">
+      <c r="L36" s="30">
         <f t="shared" si="5"/>
         <v>24929.189999999944</v>
       </c>
     </row>
     <row r="37" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E37" s="41"/>
+      <c r="E37" s="47"/>
       <c r="F37" s="27">
         <v>280</v>
       </c>
       <c r="G37" s="27"/>
       <c r="H37" s="28"/>
       <c r="I37" s="27"/>
-      <c r="J37" s="27">
+      <c r="J37" s="30">
         <f t="shared" si="3"/>
         <v>30915.159999999974</v>
       </c>
-      <c r="K37" s="27">
+      <c r="K37" s="30">
         <f t="shared" si="4"/>
         <v>164979.15999999997</v>
       </c>
-      <c r="L37" s="27">
+      <c r="L37" s="30">
         <f t="shared" si="5"/>
         <v>12519.159999999974</v>
       </c>
     </row>
     <row r="38" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E38" s="41"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="27">
         <v>290</v>
       </c>
       <c r="G38" s="27"/>
       <c r="H38" s="28"/>
       <c r="I38" s="27"/>
-      <c r="J38" s="27">
+      <c r="J38" s="30">
         <f t="shared" si="3"/>
         <v>19162.129999999946</v>
       </c>
-      <c r="K38" s="27">
+      <c r="K38" s="30">
         <f t="shared" si="4"/>
         <v>158014.12999999998</v>
       </c>
-      <c r="L38" s="27">
+      <c r="L38" s="30">
         <f t="shared" si="5"/>
         <v>109.12999999994645</v>
       </c>
     </row>
     <row r="39" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E39" s="41"/>
+      <c r="E39" s="47"/>
       <c r="F39" s="27">
         <v>300</v>
       </c>
       <c r="G39" s="27"/>
       <c r="H39" s="28"/>
       <c r="I39" s="27"/>
-      <c r="J39" s="27">
+      <c r="J39" s="30">
         <f t="shared" si="3"/>
         <v>7409.0999999999767</v>
       </c>
-      <c r="K39" s="27">
+      <c r="K39" s="30">
         <f t="shared" si="4"/>
         <v>151049.09999999998</v>
       </c>
-      <c r="L39" s="27">
+      <c r="L39" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-12300.900000000023</v>
       </c>
     </row>
     <row r="40" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E40" s="41"/>
+      <c r="E40" s="47"/>
       <c r="F40" s="27">
         <v>310</v>
       </c>
       <c r="G40" s="27"/>
       <c r="H40" s="28"/>
       <c r="I40" s="27"/>
-      <c r="J40" s="27">
+      <c r="J40" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K40" s="27">
+        <v>-4343.9300000000512</v>
+      </c>
+      <c r="K40" s="30">
         <f t="shared" si="4"/>
         <v>144084.06999999998</v>
       </c>
       <c r="L40" s="27"/>
     </row>
     <row r="41" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E41" s="41"/>
+      <c r="E41" s="47"/>
       <c r="F41" s="27">
         <v>320</v>
       </c>
@@ -4149,14 +4245,14 @@
       <c r="H41" s="28"/>
       <c r="I41" s="27"/>
       <c r="J41" s="27"/>
-      <c r="K41" s="27">
+      <c r="K41" s="30">
         <f t="shared" si="4"/>
         <v>137119.03999999998</v>
       </c>
       <c r="L41" s="27"/>
     </row>
     <row r="42" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E42" s="41"/>
+      <c r="E42" s="47"/>
       <c r="F42" s="27">
         <v>330</v>
       </c>
@@ -4164,14 +4260,14 @@
       <c r="H42" s="28"/>
       <c r="I42" s="27"/>
       <c r="J42" s="27"/>
-      <c r="K42" s="27">
+      <c r="K42" s="30">
         <f t="shared" si="4"/>
         <v>130154.00999999998</v>
       </c>
       <c r="L42" s="27"/>
     </row>
     <row r="43" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E43" s="41"/>
+      <c r="E43" s="47"/>
       <c r="F43" s="27">
         <v>340</v>
       </c>
@@ -4179,14 +4275,14 @@
       <c r="H43" s="28"/>
       <c r="I43" s="27"/>
       <c r="J43" s="27"/>
-      <c r="K43" s="27">
+      <c r="K43" s="30">
         <f t="shared" si="4"/>
         <v>123188.97999999998</v>
       </c>
       <c r="L43" s="27"/>
     </row>
     <row r="44" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E44" s="41"/>
+      <c r="E44" s="47"/>
       <c r="F44" s="27">
         <v>350</v>
       </c>
@@ -4194,14 +4290,14 @@
       <c r="H44" s="28"/>
       <c r="I44" s="27"/>
       <c r="J44" s="27"/>
-      <c r="K44" s="27">
+      <c r="K44" s="30">
         <f t="shared" si="4"/>
         <v>116223.94999999998</v>
       </c>
       <c r="L44" s="27"/>
     </row>
     <row r="45" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E45" s="41"/>
+      <c r="E45" s="47"/>
       <c r="F45" s="27">
         <v>360</v>
       </c>
@@ -4209,14 +4305,14 @@
       <c r="H45" s="28"/>
       <c r="I45" s="27"/>
       <c r="J45" s="27"/>
-      <c r="K45" s="27">
+      <c r="K45" s="30">
         <f t="shared" si="4"/>
         <v>109258.91999999998</v>
       </c>
       <c r="L45" s="27"/>
     </row>
     <row r="46" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E46" s="41"/>
+      <c r="E46" s="47"/>
       <c r="F46" s="27">
         <v>370</v>
       </c>
@@ -4224,14 +4320,14 @@
       <c r="H46" s="28"/>
       <c r="I46" s="27"/>
       <c r="J46" s="27"/>
-      <c r="K46" s="27">
+      <c r="K46" s="30">
         <f t="shared" si="4"/>
         <v>102293.88999999998</v>
       </c>
       <c r="L46" s="27"/>
     </row>
     <row r="47" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E47" s="41"/>
+      <c r="E47" s="47"/>
       <c r="F47" s="27">
         <v>380</v>
       </c>
@@ -4239,14 +4335,14 @@
       <c r="H47" s="28"/>
       <c r="I47" s="27"/>
       <c r="J47" s="27"/>
-      <c r="K47" s="27">
+      <c r="K47" s="30">
         <f t="shared" si="4"/>
         <v>95328.859999999986</v>
       </c>
       <c r="L47" s="27"/>
     </row>
     <row r="48" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E48" s="41"/>
+      <c r="E48" s="47"/>
       <c r="F48" s="27">
         <v>390</v>
       </c>
@@ -4254,14 +4350,14 @@
       <c r="H48" s="28"/>
       <c r="I48" s="27"/>
       <c r="J48" s="27"/>
-      <c r="K48" s="27">
+      <c r="K48" s="30">
         <f t="shared" si="4"/>
         <v>88363.829999999958</v>
       </c>
       <c r="L48" s="27"/>
     </row>
     <row r="49" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E49" s="41"/>
+      <c r="E49" s="47"/>
       <c r="F49" s="27">
         <v>400</v>
       </c>
@@ -4269,14 +4365,14 @@
       <c r="H49" s="28"/>
       <c r="I49" s="27"/>
       <c r="J49" s="27"/>
-      <c r="K49" s="27">
+      <c r="K49" s="30">
         <f t="shared" si="4"/>
         <v>81398.799999999988</v>
       </c>
       <c r="L49" s="27"/>
     </row>
     <row r="50" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E50" s="41"/>
+      <c r="E50" s="47"/>
       <c r="F50" s="27">
         <v>410</v>
       </c>
@@ -4284,14 +4380,14 @@
       <c r="H50" s="28"/>
       <c r="I50" s="27"/>
       <c r="J50" s="27"/>
-      <c r="K50" s="27">
+      <c r="K50" s="30">
         <f t="shared" si="4"/>
         <v>74433.76999999996</v>
       </c>
       <c r="L50" s="27"/>
     </row>
     <row r="51" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E51" s="41"/>
+      <c r="E51" s="47"/>
       <c r="F51" s="27">
         <v>420</v>
       </c>
@@ -4299,14 +4395,14 @@
       <c r="H51" s="28"/>
       <c r="I51" s="27"/>
       <c r="J51" s="27"/>
-      <c r="K51" s="27">
+      <c r="K51" s="30">
         <f t="shared" si="4"/>
         <v>67468.739999999991</v>
       </c>
       <c r="L51" s="27"/>
     </row>
     <row r="52" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E52" s="41"/>
+      <c r="E52" s="47"/>
       <c r="F52" s="27">
         <v>430</v>
       </c>
@@ -4314,14 +4410,14 @@
       <c r="H52" s="28"/>
       <c r="I52" s="27"/>
       <c r="J52" s="27"/>
-      <c r="K52" s="27">
+      <c r="K52" s="30">
         <f t="shared" si="4"/>
         <v>60503.709999999963</v>
       </c>
       <c r="L52" s="27"/>
     </row>
     <row r="53" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E53" s="41"/>
+      <c r="E53" s="47"/>
       <c r="F53" s="27">
         <v>440</v>
       </c>
@@ -4329,14 +4425,14 @@
       <c r="H53" s="28"/>
       <c r="I53" s="27"/>
       <c r="J53" s="27"/>
-      <c r="K53" s="27">
+      <c r="K53" s="30">
         <f t="shared" si="4"/>
         <v>53538.679999999993</v>
       </c>
       <c r="L53" s="27"/>
     </row>
     <row r="54" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E54" s="41"/>
+      <c r="E54" s="47"/>
       <c r="F54" s="27">
         <v>450</v>
       </c>
@@ -4344,14 +4440,14 @@
       <c r="H54" s="28"/>
       <c r="I54" s="27"/>
       <c r="J54" s="27"/>
-      <c r="K54" s="27">
+      <c r="K54" s="30">
         <f t="shared" si="4"/>
         <v>46573.649999999965</v>
       </c>
       <c r="L54" s="27"/>
     </row>
     <row r="55" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E55" s="41"/>
+      <c r="E55" s="47"/>
       <c r="F55" s="27">
         <v>460</v>
       </c>
@@ -4359,14 +4455,14 @@
       <c r="H55" s="28"/>
       <c r="I55" s="27"/>
       <c r="J55" s="27"/>
-      <c r="K55" s="27">
+      <c r="K55" s="30">
         <f t="shared" si="4"/>
         <v>39608.619999999995</v>
       </c>
       <c r="L55" s="27"/>
     </row>
     <row r="56" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E56" s="41"/>
+      <c r="E56" s="47"/>
       <c r="F56" s="27">
         <v>470</v>
       </c>
@@ -4374,14 +4470,14 @@
       <c r="H56" s="28"/>
       <c r="I56" s="27"/>
       <c r="J56" s="27"/>
-      <c r="K56" s="27">
+      <c r="K56" s="30">
         <f t="shared" si="4"/>
         <v>32643.589999999967</v>
       </c>
       <c r="L56" s="27"/>
     </row>
     <row r="57" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E57" s="41"/>
+      <c r="E57" s="47"/>
       <c r="F57" s="27">
         <v>480</v>
       </c>
@@ -4389,14 +4485,14 @@
       <c r="H57" s="28"/>
       <c r="I57" s="27"/>
       <c r="J57" s="27"/>
-      <c r="K57" s="27">
+      <c r="K57" s="30">
         <f t="shared" si="4"/>
         <v>25678.559999999998</v>
       </c>
       <c r="L57" s="27"/>
     </row>
     <row r="58" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E58" s="41"/>
+      <c r="E58" s="47"/>
       <c r="F58" s="27">
         <v>490</v>
       </c>
@@ -4404,14 +4500,14 @@
       <c r="H58" s="28"/>
       <c r="I58" s="27"/>
       <c r="J58" s="27"/>
-      <c r="K58" s="27">
+      <c r="K58" s="30">
         <f t="shared" si="4"/>
         <v>18713.52999999997</v>
       </c>
       <c r="L58" s="27"/>
     </row>
     <row r="59" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E59" s="41"/>
+      <c r="E59" s="47"/>
       <c r="F59" s="27">
         <v>500</v>
       </c>
@@ -4419,14 +4515,14 @@
       <c r="H59" s="28"/>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
-      <c r="K59" s="27">
+      <c r="K59" s="30">
         <f t="shared" si="4"/>
         <v>11748.5</v>
       </c>
       <c r="L59" s="27"/>
     </row>
     <row r="60" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E60" s="41"/>
+      <c r="E60" s="47"/>
       <c r="F60" s="27">
         <v>510</v>
       </c>
@@ -4434,14 +4530,14 @@
       <c r="H60" s="28"/>
       <c r="I60" s="27"/>
       <c r="J60" s="27"/>
-      <c r="K60" s="27">
+      <c r="K60" s="30">
         <f t="shared" si="4"/>
         <v>4783.4699999999721</v>
       </c>
       <c r="L60" s="27"/>
     </row>
     <row r="61" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E61" s="42"/>
+      <c r="E61" s="48"/>
       <c r="F61" s="27">
         <v>520</v>
       </c>
@@ -4449,9 +4545,9 @@
       <c r="H61" s="28"/>
       <c r="I61" s="27"/>
       <c r="J61" s="27"/>
-      <c r="K61" s="27">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="K61" s="30">
+        <f t="shared" si="4"/>
+        <v>-2181.5599999999977</v>
       </c>
       <c r="L61" s="27"/>
     </row>
@@ -4517,6 +4613,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B7:B8"/>
@@ -4531,10 +4631,6 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>